<commit_message>
Commit on 15/06 from Advapro
</commit_message>
<xml_diff>
--- a/TestcaseSuite.xlsx
+++ b/TestcaseSuite.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -442,269 +442,9 @@
         <v>yes</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>TC_02</v>
-      </c>
-      <c r="B3" t="str">
-        <v>2.Selecting Form Menu</v>
-      </c>
-      <c r="C3" t="str">
-        <v>click</v>
-      </c>
-      <c r="D3" t="str">
-        <v>no value</v>
-      </c>
-      <c r="E3" t="str">
-        <v>form_contains</v>
-      </c>
-      <c r="F3" t="str">
-        <v>no</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>TC_03</v>
-      </c>
-      <c r="B4" t="str">
-        <v>3.Selecting Practice forms Submenu</v>
-      </c>
-      <c r="C4" t="str">
-        <v>click</v>
-      </c>
-      <c r="D4" t="str">
-        <v>no value</v>
-      </c>
-      <c r="E4" t="str">
-        <v>practiceform_contains</v>
-      </c>
-      <c r="F4" t="str">
-        <v>no</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>TC_04</v>
-      </c>
-      <c r="B5" t="str">
-        <v>4.Entering FirstName</v>
-      </c>
-      <c r="C5" t="str">
-        <v>type</v>
-      </c>
-      <c r="D5" t="str">
-        <v>faker</v>
-      </c>
-      <c r="E5" t="str">
-        <v>first_name</v>
-      </c>
-      <c r="F5" t="str">
-        <v>no</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>TC_05</v>
-      </c>
-      <c r="B6" t="str">
-        <v>5.Entering LastName</v>
-      </c>
-      <c r="C6" t="str">
-        <v>type</v>
-      </c>
-      <c r="D6" t="str">
-        <v>faker</v>
-      </c>
-      <c r="E6" t="str">
-        <v>last_name</v>
-      </c>
-      <c r="F6" t="str">
-        <v>no</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>TC_06</v>
-      </c>
-      <c r="B7" t="str">
-        <v>6.Entering Email</v>
-      </c>
-      <c r="C7" t="str">
-        <v>type</v>
-      </c>
-      <c r="D7" t="str">
-        <v>faker</v>
-      </c>
-      <c r="E7" t="str">
-        <v>email</v>
-      </c>
-      <c r="F7" t="str">
-        <v>no</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>TC_07</v>
-      </c>
-      <c r="B8" t="str">
-        <v>7.Radiobutton Check for gender</v>
-      </c>
-      <c r="C8" t="str">
-        <v>click</v>
-      </c>
-      <c r="D8" t="str">
-        <v>no value</v>
-      </c>
-      <c r="E8" t="str">
-        <v>gender</v>
-      </c>
-      <c r="F8" t="str">
-        <v>no</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>TC_08</v>
-      </c>
-      <c r="B9" t="str">
-        <v>8.Entering Mobile number</v>
-      </c>
-      <c r="C9" t="str">
-        <v>type</v>
-      </c>
-      <c r="D9" t="str">
-        <v>faker</v>
-      </c>
-      <c r="E9" t="str">
-        <v>mobile_number</v>
-      </c>
-      <c r="F9" t="str">
-        <v>no</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>TC_09</v>
-      </c>
-      <c r="B10" t="str">
-        <v>09.Selecting Date from datepicker</v>
-      </c>
-      <c r="C10" t="str">
-        <v>date</v>
-      </c>
-      <c r="D10" t="str">
-        <v>faker</v>
-      </c>
-      <c r="E10" t="str">
-        <v>dob</v>
-      </c>
-      <c r="F10" t="str">
-        <v>no</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>TC_10</v>
-      </c>
-      <c r="B11" t="str">
-        <v xml:space="preserve">10.Scrolling to the bottom of the screen </v>
-      </c>
-      <c r="C11" t="str">
-        <v>scroll</v>
-      </c>
-      <c r="D11" t="str">
-        <v>no value</v>
-      </c>
-      <c r="E11" t="str">
-        <v>submit_contains</v>
-      </c>
-      <c r="F11" t="str">
-        <v>no</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>TC_11</v>
-      </c>
-      <c r="B12" t="str">
-        <v xml:space="preserve">11.Dynamic dropdown selection </v>
-      </c>
-      <c r="C12" t="str">
-        <v>dropdown</v>
-      </c>
-      <c r="D12" t="str">
-        <v>Com,Sc</v>
-      </c>
-      <c r="E12" t="str">
-        <v>subject</v>
-      </c>
-      <c r="F12" t="str">
-        <v>no</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v>TC_12</v>
-      </c>
-      <c r="B13" t="str">
-        <v xml:space="preserve">12.Clicking Square checkbox </v>
-      </c>
-      <c r="C13" t="str">
-        <v>click</v>
-      </c>
-      <c r="D13" t="str">
-        <v>no value</v>
-      </c>
-      <c r="E13" t="str">
-        <v>hobbies</v>
-      </c>
-      <c r="F13" t="str">
-        <v>no</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v>TC_13</v>
-      </c>
-      <c r="B14" t="str">
-        <v>13.Uploading File from windows</v>
-      </c>
-      <c r="C14" t="str">
-        <v>uploadfile</v>
-      </c>
-      <c r="D14" t="str">
-        <v>Sample image.png</v>
-      </c>
-      <c r="E14" t="str">
-        <v>upload</v>
-      </c>
-      <c r="F14" t="str">
-        <v>no</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="str">
-        <v>TC_14</v>
-      </c>
-      <c r="B15" t="str">
-        <v>14.Entering Address</v>
-      </c>
-      <c r="C15" t="str">
-        <v>type</v>
-      </c>
-      <c r="D15" t="str">
-        <v>faker</v>
-      </c>
-      <c r="E15" t="str">
-        <v>address</v>
-      </c>
-      <c r="F15" t="str">
-        <v>no</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F15"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commit to Child branch with login code
</commit_message>
<xml_diff>
--- a/TestcaseSuite.xlsx
+++ b/TestcaseSuite.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -442,9 +442,20 @@
         <v>yes</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>TC_02</v>
+      </c>
+      <c r="B3" t="str">
+        <v xml:space="preserve">Login-&gt;To Verify that Successfully landed user role-based landing page, when user Clicking on the "Adva pro Login" button. </v>
+      </c>
+      <c r="F3" t="str">
+        <v>no</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
"17/6Firstcase from Clinet project "
</commit_message>
<xml_diff>
--- a/TestcaseSuite.xlsx
+++ b/TestcaseSuite.xlsx
@@ -427,16 +427,16 @@
         <v>TC_01</v>
       </c>
       <c r="B2" t="str">
-        <v>1.Launch the browser</v>
+        <v>Login-&gt;To Verify that Successfully landed user role-based landing page, when user Clicking on the Adva pro Login button</v>
       </c>
       <c r="C2" t="str">
-        <v>openbrowser,click,click,type,type,type,click,type,date,dropdown,click,uploadfile,type</v>
+        <v>openbrowser</v>
       </c>
       <c r="D2" t="str">
-        <v>https://demoqa.com/,no value,no value,faker,faker,faker,no value,faker,faker,Com,no value,Sample image.png,faker</v>
+        <v>https://adva-pro-dev01.paradigmcentral.com</v>
       </c>
       <c r="E2" t="str">
-        <v>no value,form_contains,practiceform_contains,first_name,last_name,email,gender,mobile_number,dob,subject,hobbies,upload,address</v>
+        <v>no value</v>
       </c>
       <c r="F2" t="str">
         <v>yes</v>

</xml_diff>

<commit_message>
"First 3 working cases" 17/6
</commit_message>
<xml_diff>
--- a/TestcaseSuite.xlsx
+++ b/TestcaseSuite.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -430,21 +430,41 @@
         <v>Login-&gt;To Verify that Successfully landed user role-based landing page, when user Clicking on the Adva pro Login button</v>
       </c>
       <c r="C2" t="str">
-        <v>openbrowser</v>
+        <v>openbrowser,assert</v>
       </c>
       <c r="D2" t="str">
-        <v>https://adva-pro-dev01.paradigmcentral.com</v>
+        <v>https://adva-pro-dev01.paradigmcentral.com,https://adva-pro-dev01.paradigmcentral.com/#/providers/prospects/list</v>
       </c>
       <c r="E2" t="str">
-        <v>no value</v>
+        <v>no value,url</v>
       </c>
       <c r="F2" t="str">
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>TC_02</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Client-&gt; Create New Client screen : To verify that when the user clicks "Create" button , it navigates to the Create New Client screen</v>
+      </c>
+      <c r="C3" t="str">
+        <v>click,click,assert</v>
+      </c>
+      <c r="D3" t="str">
+        <v>no value,no value, Create New Client</v>
+      </c>
+      <c r="E3" t="str">
+        <v>client_menu,create_contains,client_text</v>
+      </c>
+      <c r="F3" t="str">
         <v>yes</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
//working code on 18/6 third cases execution
</commit_message>
<xml_diff>
--- a/TestcaseSuite.xlsx
+++ b/TestcaseSuite.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -424,7 +424,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>TC_01</v>
+        <v>140398</v>
       </c>
       <c r="B2" t="str">
         <v>Login-&gt;To Verify that Successfully landed user role-based landing page, when user Clicking on the Adva pro Login button</v>
@@ -444,7 +444,7 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>TC_02</v>
+        <v>140671</v>
       </c>
       <c r="B3" t="str">
         <v>Client-&gt; Create New Client screen : To verify that when the user clicks "Create" button , it navigates to the Create New Client screen</v>
@@ -459,12 +459,32 @@
         <v>client_menu,create_contains,client_text</v>
       </c>
       <c r="F3" t="str">
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>140688</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Client-&gt;Create Client-&gt;General Information-&gt;To verify if the user is able to click on the "Next" button and navigate to the Client information screen.</v>
+      </c>
+      <c r="C4" t="str">
+        <v>type,type,type,type,type,type,type,type,click</v>
+      </c>
+      <c r="D4" t="str">
+        <v>faker,faker,faker,faker,faker,faker,faker,faker,no value</v>
+      </c>
+      <c r="E4" t="str">
+        <v>client_name,street,city,state,zip,mobile_number,ext,website,save</v>
+      </c>
+      <c r="F4" t="str">
         <v>yes</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
5 working testcases 18/6 [cypress highlight]
</commit_message>
<xml_diff>
--- a/TestcaseSuite.xlsx
+++ b/TestcaseSuite.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -464,27 +464,67 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>140688</v>
+        <v>140741</v>
       </c>
       <c r="B4" t="str">
-        <v>Client-&gt;Create Client-&gt;General Information-&gt;To verify if the user is able to click on the "Next" button and navigate to the Client information screen.</v>
+        <v>Client-&gt;Create Client-&gt;To verify that the user can view the "Prepopulated" data in the client information screen.</v>
       </c>
       <c r="C4" t="str">
-        <v>type,type,type,type,type,type,type,type,click</v>
+        <v>type,type,type,dropdown,type,type,type,type,click</v>
       </c>
       <c r="D4" t="str">
-        <v>faker,faker,faker,faker,faker,faker,faker,faker,no value</v>
+        <v>faker,faker,faker,CA,faker,faker,faker,faker,no value</v>
       </c>
       <c r="E4" t="str">
         <v>client_name,street,city,state,zip,mobile_number,ext,website,save</v>
       </c>
       <c r="F4" t="str">
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>140688</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Client-&gt;Create Client-&gt;General Information-&gt;To verify if the user is able to click on the "Next" button and navigate to the General information screen.</v>
+      </c>
+      <c r="C5" t="str">
+        <v>click,assert</v>
+      </c>
+      <c r="D5" t="str">
+        <v xml:space="preserve">no value, 2.General Information </v>
+      </c>
+      <c r="E5" t="str">
+        <v>next,next_tab</v>
+      </c>
+      <c r="F5" t="str">
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>140728</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Client-&gt;Create Client-&gt;To verify that the user is able to navigate to the Client Summary screen after clicking the FINISH button.</v>
+      </c>
+      <c r="C6" t="str">
+        <v>click,assert</v>
+      </c>
+      <c r="D6" t="str">
+        <v>no value,Summary</v>
+      </c>
+      <c r="E6" t="str">
+        <v>finish,summary_contains</v>
+      </c>
+      <c r="F6" t="str">
         <v>yes</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commit on19/ 6 - 10 cases
</commit_message>
<xml_diff>
--- a/TestcaseSuite.xlsx
+++ b/TestcaseSuite.xlsx
@@ -610,7 +610,7 @@
         <v>Client-&gt;Client Summary-&gt;To Verify if the user can add new entries in training data.</v>
       </c>
       <c r="C11" t="str">
-        <v>type,type,click</v>
+        <v>date,type,click</v>
       </c>
       <c r="D11" t="str">
         <v>faker,faker,no value</v>
@@ -619,7 +619,7 @@
         <v>date,first_name,finish</v>
       </c>
       <c r="F11" t="str">
-        <v>no</v>
+        <v>yes</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit on 21/6 with updated xlsx
</commit_message>
<xml_diff>
--- a/TestcaseSuite.xlsx
+++ b/TestcaseSuite.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -622,9 +622,29 @@
         <v>yes</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>141287</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Client-&gt;Client Summary-&gt;Training-&gt;To verify that when the user clicks the Save button on the Client Record-Training Data screen, the data should be saved, and they should be navigated to the training main screen.</v>
+      </c>
+      <c r="C12" t="str">
+        <v>assert,click,assert,click</v>
+      </c>
+      <c r="D12" t="str">
+        <v>Trainings,no value,fixture,no value</v>
+      </c>
+      <c r="E12" t="str">
+        <v>training_assert,click_training,first_name,finish</v>
+      </c>
+      <c r="F12" t="str">
+        <v>yes</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F12"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
commit with secret [26/6/2023]
</commit_message>
<xml_diff>
--- a/TestcaseSuite.xlsx
+++ b/TestcaseSuite.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -630,21 +630,181 @@
         <v>Client-&gt;Client Summary-&gt;Training-&gt;To verify that when the user clicks the Save button on the Client Record-Training Data screen, the data should be saved, and they should be navigated to the training main screen.</v>
       </c>
       <c r="C12" t="str">
-        <v>assert,click,assert,click</v>
+        <v>assert,click,click</v>
       </c>
       <c r="D12" t="str">
-        <v>Trainings,no value,fixture,no value</v>
+        <v>Trainings,no value,no value</v>
       </c>
       <c r="E12" t="str">
-        <v>training_assert,click_training,first_name,finish</v>
+        <v>training_assert,click_training,finish</v>
       </c>
       <c r="F12" t="str">
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>141289</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Client-&gt;Client Summary-&gt;Training-&gt;To verify that the user can view previously entered training data and add new entries on the Client Record-Training Data screen.</v>
+      </c>
+      <c r="C13" t="str">
+        <v>click,date,type,click</v>
+      </c>
+      <c r="D13" t="str">
+        <v>no value,faker,faker,no value</v>
+      </c>
+      <c r="E13" t="str">
+        <v>next,date,first_name_next,cancel</v>
+      </c>
+      <c r="F13" t="str">
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>141370</v>
+      </c>
+      <c r="B14" t="str">
+        <v>To verify that the user can upload instructions by clicking the upload button.</v>
+      </c>
+      <c r="C14" t="str">
+        <v>click,click,click</v>
+      </c>
+      <c r="D14" t="str">
+        <v>no value,no value,no value</v>
+      </c>
+      <c r="E14" t="str">
+        <v>instruction,next,close_popup</v>
+      </c>
+      <c r="F14" t="str">
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>144229</v>
+      </c>
+      <c r="B15" t="str">
+        <v>To verify that the existing summary page displays a detailed view of all the tabs in the Summary Page.</v>
+      </c>
+      <c r="C15" t="str">
+        <v>click</v>
+      </c>
+      <c r="D15" t="str">
+        <v>no value</v>
+      </c>
+      <c r="E15" t="str">
+        <v>training</v>
+      </c>
+      <c r="F15" t="str">
+        <v>no</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>141406</v>
+      </c>
+      <c r="B16" t="str">
+        <v>Client-Client Summary-Activity log-&gt;To verify if the correct action of the user mentioned in the FRD (Record updated, Case manager assigned, Status changed, Referral created, comments added, documents uploaded) is displayed in the Activity log.</v>
+      </c>
+      <c r="C16" t="str">
+        <v>click</v>
+      </c>
+      <c r="D16" t="str">
+        <v>no value</v>
+      </c>
+      <c r="E16" t="str">
+        <v>document</v>
+      </c>
+      <c r="F16" t="str">
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>141340</v>
+      </c>
+      <c r="B17" t="str">
+        <v>To verify that each document should have at least one tag in the Upload document pop-up.</v>
+      </c>
+      <c r="C17" t="str">
+        <v>click</v>
+      </c>
+      <c r="D17" t="str">
+        <v>no value</v>
+      </c>
+      <c r="E17" t="str">
+        <v>instruction</v>
+      </c>
+      <c r="F17" t="str">
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>141370</v>
+      </c>
+      <c r="B18" t="str">
+        <v>Client-Client Summary-&gt;Instruction-&gt;To verify that the user can upload instructions by clicking the upload button.</v>
+      </c>
+      <c r="C18" t="str">
+        <v>click</v>
+      </c>
+      <c r="D18" t="str">
+        <v>no value</v>
+      </c>
+      <c r="E18" t="str">
+        <v>training</v>
+      </c>
+      <c r="F18" t="str">
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>141380</v>
+      </c>
+      <c r="B19" t="str">
+        <v>Client-&gt;Client Summary-&gt;Instruction-&gt;To verify that if there is no data in the instruction section, the error message "No record found" is displayed.</v>
+      </c>
+      <c r="C19" t="str">
+        <v>click</v>
+      </c>
+      <c r="D19" t="str">
+        <v>no value</v>
+      </c>
+      <c r="E19" t="str">
+        <v>document</v>
+      </c>
+      <c r="F19" t="str">
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>141406</v>
+      </c>
+      <c r="B20" t="str">
+        <v>Client-Client Summary-Activity log-&gt;To verify if the correct action of the user mentioned in the FRD (Record updated, Case manager assigned, Status changed, Referral created, comments added, documents uploaded) is displayed in the Activity log.</v>
+      </c>
+      <c r="C20" t="str">
+        <v>click</v>
+      </c>
+      <c r="D20" t="str">
+        <v>no value</v>
+      </c>
+      <c r="E20" t="str">
+        <v>instruction</v>
+      </c>
+      <c r="F20" t="str">
         <v>yes</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F12"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F20"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commit on Recent changes[28/6]
</commit_message>
<xml_diff>
--- a/TestcaseSuite.xlsx
+++ b/TestcaseSuite.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -719,7 +719,7 @@
         <v>document</v>
       </c>
       <c r="F16" t="str">
-        <v>yes</v>
+        <v>no</v>
       </c>
     </row>
     <row r="17">
@@ -739,15 +739,15 @@
         <v>instruction</v>
       </c>
       <c r="F17" t="str">
-        <v>yes</v>
+        <v>no</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>141370</v>
+        <v>141380</v>
       </c>
       <c r="B18" t="str">
-        <v>Client-Client Summary-&gt;Instruction-&gt;To verify that the user can upload instructions by clicking the upload button.</v>
+        <v>Client-&gt;Client Summary-&gt;Instruction-&gt;To verify that if there is no data in the instruction section, the error message "No record found" is displayed.</v>
       </c>
       <c r="C18" t="str">
         <v>click</v>
@@ -756,55 +756,15 @@
         <v>no value</v>
       </c>
       <c r="E18" t="str">
-        <v>training</v>
+        <v>document</v>
       </c>
       <c r="F18" t="str">
-        <v>yes</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="str">
-        <v>141380</v>
-      </c>
-      <c r="B19" t="str">
-        <v>Client-&gt;Client Summary-&gt;Instruction-&gt;To verify that if there is no data in the instruction section, the error message "No record found" is displayed.</v>
-      </c>
-      <c r="C19" t="str">
-        <v>click</v>
-      </c>
-      <c r="D19" t="str">
-        <v>no value</v>
-      </c>
-      <c r="E19" t="str">
-        <v>document</v>
-      </c>
-      <c r="F19" t="str">
-        <v>yes</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="str">
-        <v>141406</v>
-      </c>
-      <c r="B20" t="str">
-        <v>Client-Client Summary-Activity log-&gt;To verify if the correct action of the user mentioned in the FRD (Record updated, Case manager assigned, Status changed, Referral created, comments added, documents uploaded) is displayed in the Activity log.</v>
-      </c>
-      <c r="C20" t="str">
-        <v>click</v>
-      </c>
-      <c r="D20" t="str">
-        <v>no value</v>
-      </c>
-      <c r="E20" t="str">
-        <v>instruction</v>
-      </c>
-      <c r="F20" t="str">
-        <v>yes</v>
+        <v>no</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F20"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F18"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>